<commit_message>
Correção de erros no Excel
</commit_message>
<xml_diff>
--- a/resources/cdm/cdm_fazeconta.xlsx
+++ b/resources/cdm/cdm_fazeconta.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="151">
   <si>
     <t>table_name</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>id do aluno associado ao responsável</t>
-  </si>
-  <si>
-    <t>07.01.2025: removed fields with column names: data_admissao e data_renovacao (AC)</t>
   </si>
   <si>
     <t>vac_id</t>
@@ -505,7 +502,7 @@
   <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -523,6 +520,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -552,12 +555,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -726,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -737,29 +746,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1294,134 +1304,134 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="24" t="s">
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="26" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="C2" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="26" t="s">
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="26" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="C4" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="25" t="s">
+      <c r="C6" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="27" t="s">
+      <c r="C7" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="C8" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="C8" s="25" t="s">
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="C9" s="27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="C9" s="26" t="s">
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="C10" s="26" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="C10" s="25" t="s">
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="C11" s="27" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="26" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="C12" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="C13" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="C12" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="C13" s="26" t="s">
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="C14" s="26" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="C14" s="25" t="s">
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="C15" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="C16" s="26" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="C15" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="C16" s="25" t="s">
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="C17" s="27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="C17" s="26" t="s">
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="C18" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="C19" s="27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="C18" s="25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="C19" s="26" t="s">
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="C20" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="C21" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="26" t="s">
+    <row r="22" ht="12.5" customHeight="1">
+      <c r="C22" s="29" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="22" ht="12.5" customHeight="1">
-      <c r="C22" s="28" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1446,7 @@
   <sheetPr enableFormatConditionsCalculation="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="true"/>
   </sheetViews>
@@ -1810,7 +1820,6 @@
     </row>
     <row r="23" ht="12.5" customHeight="1">
       <c r="B23" s="2"/>
-      <c r="C23" s="5"/>
       <c r="D23" s="4"/>
       <c r="E23" s="2"/>
     </row>
@@ -1840,14 +1849,10 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" ht="12.5" customHeight="1">
-      <c r="B29" s="2"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="2"/>
     </row>
     <row r="30" ht="12.5" customHeight="1">
-      <c r="B30" s="2"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="2"/>
     </row>
     <row r="31" ht="12.5" customHeight="1">
       <c r="D31" s="4"/>
@@ -4753,15 +4758,9 @@
     <row r="998" ht="12.5" customHeight="1">
       <c r="D998" s="4"/>
     </row>
-    <row r="999" ht="12.5" customHeight="1">
-      <c r="D999" s="4"/>
-    </row>
-    <row r="1000" ht="12.5" customHeight="1">
-      <c r="D1000" s="4"/>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z1000"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z998"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4771,7 +4770,7 @@
   <sheetPr enableFormatConditionsCalculation="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z986"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="true"/>
   </sheetViews>
@@ -4891,10 +4890,10 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="4"/>
@@ -4930,10 +4929,10 @@
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="4"/>
@@ -4942,10 +4941,10 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="4"/>
@@ -5107,15 +5106,15 @@
       </c>
     </row>
     <row r="20" ht="12.5" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -5123,44 +5122,28 @@
       </c>
     </row>
     <row r="21" ht="12.5" customHeight="1">
-      <c r="B21" s="2"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="2"/>
     </row>
     <row r="22" ht="12.5" customHeight="1">
-      <c r="B22" s="2"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="2"/>
     </row>
     <row r="23" ht="12.5" customHeight="1">
-      <c r="B23" s="2"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="2"/>
     </row>
     <row r="24" ht="12.5" customHeight="1">
-      <c r="B24" s="2"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="2"/>
     </row>
     <row r="25" ht="12.5" customHeight="1">
-      <c r="B25" s="2"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="2"/>
     </row>
     <row r="26" ht="12.5" customHeight="1">
-      <c r="B26" s="2"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="2"/>
     </row>
     <row r="27" ht="12.5" customHeight="1">
-      <c r="B27" s="2"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="2"/>
     </row>
     <row r="28" ht="12.5" customHeight="1">
-      <c r="B28" s="2"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="2"/>
     </row>
     <row r="29" ht="12.5" customHeight="1">
       <c r="D29" s="4"/>
@@ -5173,9 +5156,6 @@
     </row>
     <row r="32" ht="12.5" customHeight="1">
       <c r="D32" s="4"/>
-      <c r="G32" s="2" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="33" ht="12.5" customHeight="1">
       <c r="D33" s="4"/>
@@ -8039,45 +8019,9 @@
     <row r="986" ht="12.5" customHeight="1">
       <c r="D986" s="4"/>
     </row>
-    <row r="987" ht="12.5" customHeight="1">
-      <c r="D987" s="4"/>
-    </row>
-    <row r="988" ht="12.5" customHeight="1">
-      <c r="D988" s="4"/>
-    </row>
-    <row r="989" ht="12.5" customHeight="1">
-      <c r="D989" s="4"/>
-    </row>
-    <row r="990" ht="12.5" customHeight="1">
-      <c r="D990" s="4"/>
-    </row>
-    <row r="991" ht="12.5" customHeight="1">
-      <c r="D991" s="4"/>
-    </row>
-    <row r="992" ht="12.5" customHeight="1">
-      <c r="D992" s="4"/>
-    </row>
-    <row r="993" ht="12.5" customHeight="1">
-      <c r="D993" s="4"/>
-    </row>
-    <row r="994" ht="12.5" customHeight="1">
-      <c r="D994" s="4"/>
-    </row>
-    <row r="995" ht="12.5" customHeight="1">
-      <c r="D995" s="4"/>
-    </row>
-    <row r="996" ht="12.5" customHeight="1">
-      <c r="D996" s="4"/>
-    </row>
-    <row r="997" ht="12.5" customHeight="1">
-      <c r="D997" s="4"/>
-    </row>
-    <row r="998" ht="12.5" customHeight="1">
-      <c r="D998" s="4"/>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Z998"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z986"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8164,7 +8108,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -8190,7 +8134,7 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -8205,7 +8149,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>28</v>
@@ -8219,11 +8163,11 @@
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="2" t="s">
@@ -11364,7 +11308,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -11391,10 +11335,10 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
@@ -11407,10 +11351,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
@@ -11422,7 +11366,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -11437,7 +11381,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
@@ -14578,7 +14522,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -14592,7 +14536,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
@@ -14607,10 +14551,10 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
@@ -14620,7 +14564,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>
@@ -14635,7 +14579,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
@@ -17777,7 +17721,7 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -17791,7 +17735,7 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>53</v>
@@ -17804,10 +17748,10 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4"/>
@@ -17817,7 +17761,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>22</v>
@@ -17832,7 +17776,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
@@ -17845,7 +17789,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
@@ -17858,10 +17802,10 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
@@ -21007,7 +20951,7 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -24094,432 +24038,432 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="10">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="9">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="11" t="s">
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="13" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="12" t="s">
+      <c r="B4" s="14">
+        <v>358.76</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="13">
-        <v>358.76</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="B5" s="15">
+        <v>637.45</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="14">
-        <v>637.45</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="B6" s="14">
+        <f>ROUND(129.756006089531,2)</f>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="13">
-        <f>ROUND(129.756006089531,2)</f>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="B7" s="15">
+        <v>112.11275652173002</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="14">
-        <v>112.11275652173002</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="15" t="s">
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="12" t="s">
+      <c r="B9" s="14">
+        <v>1199.6702689740764</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="13">
-        <v>1199.6702689740764</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="12" t="s">
+      <c r="B10" s="14">
+        <v>95.75449341834513</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="13">
-        <v>95.75449341834513</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="12" t="s">
+      <c r="B11" s="14">
+        <v>1409.0133953186307</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="13">
-        <v>1409.0133953186307</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
+      <c r="B12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B13" s="14">
+        <v>725.1615799542411</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="13">
-        <v>725.1615799542411</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="12" t="s">
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B15" s="14">
+        <v>1512.0964581536675</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="14">
+        <v>197.376397611229</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="15">
+        <v>78.16844934721331</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="14">
+        <v>225.03537525758549</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="14">
+        <v>78.1845102705213</v>
+      </c>
+    </row>
+    <row r="20" ht="14.5" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="14">
+        <v>642.3630567893651</v>
+      </c>
+    </row>
+    <row r="21" ht="14.5" customHeight="1">
+      <c r="A21" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="14">
+        <v>23.85505455319776</v>
+      </c>
+    </row>
+    <row r="22" ht="14.5" customHeight="1">
+      <c r="A22" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" ht="14.5" customHeight="1">
+      <c r="A23" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2627.869015131001</v>
+      </c>
+    </row>
+    <row r="24" ht="14.5" customHeight="1">
+      <c r="A24" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="14">
+        <v>7204.06388045407</v>
+      </c>
+    </row>
+    <row r="25" ht="14.5" customHeight="1">
+      <c r="A25" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="13">
-        <v>1512.0964581536675</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" s="13">
-        <v>197.376397611229</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B17" s="14">
-        <v>78.16844934721331</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="13">
-        <v>225.03537525758549</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="13">
-        <v>78.1845102705213</v>
-      </c>
-    </row>
-    <row r="20" ht="14.5" customHeight="1">
-      <c r="A20" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="13">
-        <v>642.3630567893651</v>
-      </c>
-    </row>
-    <row r="21" ht="14.5" customHeight="1">
-      <c r="A21" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="13">
-        <v>23.85505455319776</v>
-      </c>
-    </row>
-    <row r="22" ht="14.5" customHeight="1">
-      <c r="A22" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="11"/>
-    </row>
-    <row r="23" ht="14.5" customHeight="1">
-      <c r="A23" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" s="13">
-        <v>2627.869015131001</v>
-      </c>
-    </row>
-    <row r="24" ht="14.5" customHeight="1">
-      <c r="A24" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="13">
-        <v>7204.06388045407</v>
-      </c>
-    </row>
-    <row r="25" ht="14.5" customHeight="1">
-      <c r="A25" s="12" t="s">
+    <row r="26" ht="14.5" customHeight="1">
+      <c r="A26" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B26" s="14">
+        <v>271.87724220918534</v>
+      </c>
+    </row>
+    <row r="27" ht="14.5" customHeight="1">
+      <c r="A27" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="14">
+        <v>1828.97690125786</v>
+      </c>
+    </row>
+    <row r="28" ht="14.5" customHeight="1">
+      <c r="A28" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="14">
+        <v>19618.378816839908</v>
+      </c>
+    </row>
+    <row r="29" ht="14.5" customHeight="1">
+      <c r="A29" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="26" ht="14.5" customHeight="1">
-      <c r="A26" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" s="13">
-        <v>271.87724220918534</v>
-      </c>
-    </row>
-    <row r="27" ht="14.5" customHeight="1">
-      <c r="A27" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="13">
-        <v>1828.97690125786</v>
-      </c>
-    </row>
-    <row r="28" ht="14.5" customHeight="1">
-      <c r="A28" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28" s="13">
-        <v>19618.378816839908</v>
-      </c>
-    </row>
-    <row r="29" ht="14.5" customHeight="1">
-      <c r="A29" s="12" t="s">
+    <row r="30" ht="14.5" customHeight="1">
+      <c r="A30" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" ht="14.5" customHeight="1">
+      <c r="A31" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="14">
+        <v>152.1464453616283</v>
+      </c>
+    </row>
+    <row r="32" ht="14.5" customHeight="1">
+      <c r="A32" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="14">
+        <v>465.5699711942172</v>
+      </c>
+    </row>
+    <row r="33" ht="14.5" customHeight="1">
+      <c r="A33" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="14">
+        <v>308.00970883541794</v>
+      </c>
+    </row>
+    <row r="34" ht="14.5" customHeight="1">
+      <c r="A34" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="14">
+        <v>376.76787854667873</v>
+      </c>
+    </row>
+    <row r="35" ht="14.5" customHeight="1">
+      <c r="A35" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="14">
+        <v>374.35771547812743</v>
+      </c>
+    </row>
+    <row r="36" ht="14.5" customHeight="1">
+      <c r="A36" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="12"/>
+    </row>
+    <row r="37" ht="14.5" customHeight="1">
+      <c r="A37" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="30" ht="14.5" customHeight="1">
-      <c r="A30" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B30" s="11"/>
-    </row>
-    <row r="31" ht="14.5" customHeight="1">
-      <c r="A31" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B31" s="13">
-        <v>152.1464453616283</v>
-      </c>
-    </row>
-    <row r="32" ht="14.5" customHeight="1">
-      <c r="A32" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B32" s="13">
-        <v>465.5699711942172</v>
-      </c>
-    </row>
-    <row r="33" ht="14.5" customHeight="1">
-      <c r="A33" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" s="13">
-        <v>308.00970883541794</v>
-      </c>
-    </row>
-    <row r="34" ht="14.5" customHeight="1">
-      <c r="A34" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B34" s="13">
-        <v>376.76787854667873</v>
-      </c>
-    </row>
-    <row r="35" ht="14.5" customHeight="1">
-      <c r="A35" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B35" s="13">
-        <v>374.35771547812743</v>
-      </c>
-    </row>
-    <row r="36" ht="14.5" customHeight="1">
-      <c r="A36" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B36" s="11"/>
-    </row>
-    <row r="37" ht="14.5" customHeight="1">
-      <c r="A37" s="12" t="s">
+    <row r="38" ht="14.5" customHeight="1">
+      <c r="A38" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B38" s="14">
+        <v>249.07007497631042</v>
+      </c>
+    </row>
+    <row r="39" ht="14.5" customHeight="1">
+      <c r="A39" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="38" ht="14.5" customHeight="1">
-      <c r="A38" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" s="13">
-        <v>249.07007497631042</v>
-      </c>
-    </row>
-    <row r="39" ht="14.5" customHeight="1">
-      <c r="A39" s="12" t="s">
+    <row r="40" ht="14.5" customHeight="1">
+      <c r="A40" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B40" s="14">
+        <v>824.6164332674277</v>
+      </c>
+    </row>
+    <row r="41" ht="14.5" customHeight="1">
+      <c r="A41" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="40" ht="14.5" customHeight="1">
-      <c r="A40" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="13">
-        <v>824.6164332674277</v>
-      </c>
-    </row>
-    <row r="41" ht="14.5" customHeight="1">
-      <c r="A41" s="12" t="s">
+    <row r="42" ht="14.5" customHeight="1">
+      <c r="A42" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B42" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="42" ht="14.5" customHeight="1">
-      <c r="A42" s="12" t="s">
+    <row r="43" ht="14.5" customHeight="1">
+      <c r="A43" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="13">
+      <c r="B43" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="43" ht="14.5" customHeight="1">
-      <c r="A43" s="12" t="s">
+    <row r="44" ht="14.5" customHeight="1">
+      <c r="A44" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B44" s="14">
+        <v>300.9048231274185</v>
+      </c>
+    </row>
+    <row r="45" ht="14.5" customHeight="1">
+      <c r="A45" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="14">
+        <v>293.6328331912812</v>
+      </c>
+    </row>
+    <row r="46" ht="14.5" customHeight="1">
+      <c r="A46" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="44" ht="14.5" customHeight="1">
-      <c r="A44" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B44" s="13">
-        <v>300.9048231274185</v>
-      </c>
-    </row>
-    <row r="45" ht="14.5" customHeight="1">
-      <c r="A45" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B45" s="13">
-        <v>293.6328331912812</v>
-      </c>
-    </row>
-    <row r="46" ht="14.5" customHeight="1">
-      <c r="A46" s="19" t="s">
+    <row r="47" ht="14.5" customHeight="1">
+      <c r="A47" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B47" s="14">
+        <v>1066.5108224346195</v>
+      </c>
+    </row>
+    <row r="48" ht="14.5" customHeight="1">
+      <c r="A48" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="14">
+        <v>357.19008213084146</v>
+      </c>
+    </row>
+    <row r="49" ht="14.5" customHeight="1">
+      <c r="A49" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" s="21">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" ht="14.5" customHeight="1">
-      <c r="A47" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="13">
-        <v>1066.5108224346195</v>
-      </c>
-    </row>
-    <row r="48" ht="14.5" customHeight="1">
-      <c r="A48" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B48" s="13">
-        <v>357.19008213084146</v>
-      </c>
-    </row>
-    <row r="49" ht="14.5" customHeight="1">
-      <c r="A49" s="12" t="s">
+      <c r="C49" s="22"/>
+    </row>
+    <row r="50" ht="14.5" customHeight="1">
+      <c r="A50" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B50" s="21">
         <v>0</v>
       </c>
-      <c r="C49" s="21"/>
-    </row>
-    <row r="50" ht="14.5" customHeight="1">
-      <c r="A50" s="12" t="s">
+      <c r="C50" s="23"/>
+    </row>
+    <row r="51" ht="14.5" customHeight="1">
+      <c r="A51" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B51" s="21">
         <v>0</v>
       </c>
-      <c r="C50" s="22"/>
-    </row>
-    <row r="51" ht="14.5" customHeight="1">
-      <c r="A51" s="12" t="s">
+      <c r="C51" s="22"/>
+    </row>
+    <row r="52" ht="14.5" customHeight="1">
+      <c r="A52" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B52" s="21">
+        <v>1083.6460410670754</v>
+      </c>
+      <c r="C52" s="22"/>
+    </row>
+    <row r="53" ht="14.5" customHeight="1">
+      <c r="A53" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="14">
         <v>0</v>
       </c>
-      <c r="C51" s="21"/>
-    </row>
-    <row r="52" ht="14.5" customHeight="1">
-      <c r="A52" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B52" s="20">
-        <v>1083.6460410670754</v>
-      </c>
-      <c r="C52" s="21"/>
-    </row>
-    <row r="53" ht="14.5" customHeight="1">
-      <c r="A53" s="12" t="s">
+    </row>
+    <row r="54" ht="13" customHeight="1">
+      <c r="A54" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B53" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" ht="13" customHeight="1">
-      <c r="A54" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B54" s="13">
+      <c r="B54" s="14">
         <v>40.64712181231429</v>
       </c>
     </row>
     <row r="55" ht="14.5" customHeight="1">
-      <c r="A55" s="7"/>
-      <c r="B55" s="23">
+      <c r="A55" s="8"/>
+      <c r="B55" s="24">
         <v>44794.886414924586</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Report Alunos por sala
</commit_message>
<xml_diff>
--- a/resources/cdm/cdm_fazeconta.xlsx
+++ b/resources/cdm/cdm_fazeconta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berna\OneDrive\Documentos\GitHub\faz-e-conta\resources\cdm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C501C-0F02-43DC-8BB6-99A2DAA71D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE5CE4A-5385-4558-9546-A3AA4CF83684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Summary" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="Suppl" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="264">
   <si>
     <t>table_name</t>
   </si>
@@ -220,9 +221,6 @@
   </si>
   <si>
     <t>Sala</t>
-  </si>
-  <si>
-    <t>func_id</t>
   </si>
   <si>
     <t>Y</t>
@@ -531,9 +529,6 @@
     <t>Valência</t>
   </si>
   <si>
-    <t>ma_id</t>
-  </si>
-  <si>
     <t>Aluno ID</t>
   </si>
   <si>
@@ -583,9 +578,6 @@
   </si>
   <si>
     <t>Descrição de acordo de pagamento entre escola e responsável educativo</t>
-  </si>
-  <si>
-    <t>mss_id</t>
   </si>
   <si>
     <t>mensalidade_valor</t>
@@ -845,6 +837,12 @@
   <si>
     <t>aluno_financas_id</t>
   </si>
+  <si>
+    <t>mensalidade_aluno_id</t>
+  </si>
+  <si>
+    <t>comparticipacao_mensal_ss_id</t>
+  </si>
 </sst>
 </file>
 
@@ -1059,7 +1057,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1109,7 +1107,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1454,11 +1451,11 @@
   </sheetPr>
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.5" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
@@ -1613,7 +1610,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Y11 A13:Y21 B12:Y12" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:Y11 A13:Y14 B12:Y12 A16:Y21 C15:Y15" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1629,7 +1626,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -1688,7 +1685,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
@@ -1697,13 +1694,13 @@
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
@@ -1712,7 +1709,7 @@
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -1727,7 +1724,7 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
@@ -1739,7 +1736,7 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -4749,7 +4746,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -4781,7 +4778,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -4817,12 +4814,12 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -4832,12 +4829,12 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -4847,12 +4844,12 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -4862,25 +4859,25 @@
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7884,7 +7881,7 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -7916,7 +7913,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -7940,7 +7937,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -7952,12 +7949,12 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -7967,7 +7964,7 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7978,7 +7975,7 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
@@ -7987,7 +7984,7 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -8002,7 +7999,7 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
@@ -8012,12 +8009,12 @@
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
@@ -8027,12 +8024,12 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
@@ -8042,12 +8039,12 @@
         <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
@@ -8057,12 +8054,12 @@
         <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -8072,12 +8069,12 @@
         <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
@@ -8087,12 +8084,12 @@
         <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
@@ -8102,12 +8099,12 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
@@ -8117,12 +8114,12 @@
         <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
@@ -8132,12 +8129,12 @@
         <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
@@ -8147,7 +8144,7 @@
         <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11120,9 +11117,11 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -11154,7 +11153,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -11190,12 +11189,12 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -11205,12 +11204,12 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -11220,12 +11219,12 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -11235,25 +11234,25 @@
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14241,7 +14240,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Z1000" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:Z5 A7:Z1000 B6:Z6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -14253,11 +14252,13 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
@@ -14287,7 +14288,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -14311,7 +14312,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -14323,7 +14324,7 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14334,67 +14335,67 @@
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
@@ -14404,12 +14405,12 @@
         <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
@@ -14419,12 +14420,12 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
@@ -14434,27 +14435,27 @@
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
@@ -14464,12 +14465,12 @@
         <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
@@ -14479,7 +14480,7 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -17456,7 +17457,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Z1003" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:Z1 A3:Z1003 B2:Z2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -17468,11 +17469,13 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
@@ -17502,7 +17505,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -17526,7 +17529,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>178</v>
+        <v>263</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -17536,7 +17539,7 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -17551,12 +17554,12 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
         <v>55</v>
@@ -17566,109 +17569,121 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="s">
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>172</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
         <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" t="s">
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -20641,7 +20656,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Z1001" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:Z1 A3:Z6 B2:Z2 A11:Z1001 A7 C7:Z7 A8 C8:Z8 A9 C9:Z9 A10 C10:Z10" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -20655,7 +20670,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="3" width="12.5" customWidth="1"/>
@@ -20663,7 +20678,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="5"/>
     </row>
@@ -20675,15 +20690,15 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B4" s="10">
         <v>358.76</v>
@@ -20691,7 +20706,7 @@
     </row>
     <row r="5" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B5" s="11">
         <v>637.45000000000005</v>
@@ -20699,7 +20714,7 @@
     </row>
     <row r="6" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B6" s="10">
         <f>ROUND(129.756006089531,2)</f>
@@ -20708,7 +20723,7 @@
     </row>
     <row r="7" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B7" s="11">
         <v>112.11275652173002</v>
@@ -20716,13 +20731,13 @@
     </row>
     <row r="8" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B9" s="10">
         <v>1199.6702689740764</v>
@@ -20730,7 +20745,7 @@
     </row>
     <row r="10" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B10" s="10">
         <v>95.754493418345135</v>
@@ -20738,7 +20753,7 @@
     </row>
     <row r="11" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B11" s="10">
         <v>1409.0133953186307</v>
@@ -20746,7 +20761,7 @@
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B12" s="10">
         <v>0</v>
@@ -20754,7 +20769,7 @@
     </row>
     <row r="13" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B13" s="10">
         <v>725.16157995424112</v>
@@ -20762,7 +20777,7 @@
     </row>
     <row r="14" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B14" s="10">
         <v>0</v>
@@ -20770,7 +20785,7 @@
     </row>
     <row r="15" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B15" s="10">
         <v>1512.0964581536675</v>
@@ -20778,7 +20793,7 @@
     </row>
     <row r="16" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B16" s="10">
         <v>197.37639761122901</v>
@@ -20786,7 +20801,7 @@
     </row>
     <row r="17" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B17" s="11">
         <v>78.168449347213311</v>
@@ -20794,7 +20809,7 @@
     </row>
     <row r="18" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B18" s="10">
         <v>225.03537525758549</v>
@@ -20802,7 +20817,7 @@
     </row>
     <row r="19" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B19" s="10">
         <v>78.184510270521301</v>
@@ -20810,7 +20825,7 @@
     </row>
     <row r="20" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B20" s="10">
         <v>642.36305678936515</v>
@@ -20818,7 +20833,7 @@
     </row>
     <row r="21" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B21" s="10">
         <v>23.85505455319776</v>
@@ -20826,13 +20841,13 @@
     </row>
     <row r="22" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B22" s="8"/>
     </row>
     <row r="23" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B23" s="10">
         <v>2627.8690151310011</v>
@@ -20840,7 +20855,7 @@
     </row>
     <row r="24" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B24" s="10">
         <v>7204.0638804540704</v>
@@ -20848,7 +20863,7 @@
     </row>
     <row r="25" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B25" s="10">
         <v>0</v>
@@ -20856,7 +20871,7 @@
     </row>
     <row r="26" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B26" s="10">
         <v>271.87724220918534</v>
@@ -20864,7 +20879,7 @@
     </row>
     <row r="27" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B27" s="10">
         <v>1828.9769012578599</v>
@@ -20872,7 +20887,7 @@
     </row>
     <row r="28" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B28" s="10">
         <v>19618.378816839908</v>
@@ -20880,7 +20895,7 @@
     </row>
     <row r="29" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B29" s="10">
         <v>0</v>
@@ -20888,13 +20903,13 @@
     </row>
     <row r="30" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B30" s="8"/>
     </row>
     <row r="31" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B31" s="10">
         <v>152.14644536162831</v>
@@ -20902,7 +20917,7 @@
     </row>
     <row r="32" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B32" s="10">
         <v>465.5699711942172</v>
@@ -20910,7 +20925,7 @@
     </row>
     <row r="33" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B33" s="10">
         <v>308.00970883541794</v>
@@ -20918,7 +20933,7 @@
     </row>
     <row r="34" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B34" s="10">
         <v>376.76787854667873</v>
@@ -20926,7 +20941,7 @@
     </row>
     <row r="35" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B35" s="10">
         <v>374.35771547812743</v>
@@ -20934,13 +20949,13 @@
     </row>
     <row r="36" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B36" s="8"/>
     </row>
     <row r="37" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B37" s="10">
         <v>0</v>
@@ -20948,7 +20963,7 @@
     </row>
     <row r="38" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B38" s="10">
         <v>249.07007497631042</v>
@@ -20956,7 +20971,7 @@
     </row>
     <row r="39" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B39" s="10">
         <v>0</v>
@@ -20964,7 +20979,7 @@
     </row>
     <row r="40" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B40" s="10">
         <v>824.61643326742774</v>
@@ -20972,7 +20987,7 @@
     </row>
     <row r="41" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B41" s="10">
         <v>0</v>
@@ -20980,7 +20995,7 @@
     </row>
     <row r="42" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B42" s="10">
         <v>0</v>
@@ -20988,7 +21003,7 @@
     </row>
     <row r="43" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B43" s="10">
         <v>0</v>
@@ -20996,7 +21011,7 @@
     </row>
     <row r="44" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B44" s="10">
         <v>300.90482312741852</v>
@@ -21004,7 +21019,7 @@
     </row>
     <row r="45" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B45" s="10">
         <v>293.63283319128118</v>
@@ -21012,7 +21027,7 @@
     </row>
     <row r="46" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B46" s="10">
         <v>0</v>
@@ -21020,7 +21035,7 @@
     </row>
     <row r="47" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B47" s="10">
         <v>1066.5108224346195</v>
@@ -21028,7 +21043,7 @@
     </row>
     <row r="48" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B48" s="10">
         <v>357.19008213084146</v>
@@ -21036,7 +21051,7 @@
     </row>
     <row r="49" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B49" s="17">
         <v>0</v>
@@ -21045,7 +21060,7 @@
     </row>
     <row r="50" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B50" s="17">
         <v>0</v>
@@ -21054,7 +21069,7 @@
     </row>
     <row r="51" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B51" s="17">
         <v>0</v>
@@ -21063,7 +21078,7 @@
     </row>
     <row r="52" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B52" s="17">
         <v>1083.6460410670754</v>
@@ -21072,7 +21087,7 @@
     </row>
     <row r="53" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B53" s="10">
         <v>0</v>
@@ -21080,7 +21095,7 @@
     </row>
     <row r="54" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B54" s="10">
         <v>40.647121812314289</v>
@@ -22057,7 +22072,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.75" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
@@ -22066,15 +22081,15 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>24</v>
@@ -22082,15 +22097,15 @@
     </row>
     <row r="3" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>31</v>
@@ -22106,15 +22121,15 @@
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>37</v>
@@ -22122,37 +22137,37 @@
     </row>
     <row r="8" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="23" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C9" s="24" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="24" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="24" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="23" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -22162,22 +22177,22 @@
     </row>
     <row r="16" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="23" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="24" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="3:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="3:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C19" s="24" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="3:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -22187,12 +22202,12 @@
     </row>
     <row r="21" spans="3:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="24" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="3:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="26" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -22214,7 +22229,7 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -25541,7 +25556,7 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -25597,7 +25612,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -25609,10 +25624,10 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
         <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25629,7 +25644,7 @@
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25646,7 +25661,7 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25654,18 +25669,18 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -25677,12 +25692,12 @@
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -25694,7 +25709,7 @@
         <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25702,13 +25717,13 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25722,7 +25737,7 @@
         <v>26</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25736,7 +25751,7 @@
         <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25750,7 +25765,7 @@
         <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25764,7 +25779,7 @@
         <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25778,12 +25793,12 @@
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
@@ -25792,12 +25807,12 @@
         <v>34</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
@@ -25806,26 +25821,26 @@
         <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
         <v>78</v>
-      </c>
-      <c r="B16" t="s">
-        <v>79</v>
       </c>
       <c r="E16" t="s">
         <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
@@ -25834,7 +25849,7 @@
         <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -25845,59 +25860,59 @@
         <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
       <c r="F19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" t="s">
         <v>86</v>
-      </c>
-      <c r="G19" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -28856,11 +28871,11 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="B6" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.58203125" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -28892,7 +28907,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -28916,7 +28931,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -28963,7 +28978,7 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
@@ -29002,7 +29017,7 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
@@ -29098,7 +29113,7 @@
     </row>
     <row r="15" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
@@ -29110,7 +29125,7 @@
     </row>
     <row r="16" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
@@ -29125,7 +29140,7 @@
     </row>
     <row r="17" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
@@ -29143,7 +29158,7 @@
     </row>
     <row r="18" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
@@ -29161,10 +29176,10 @@
     </row>
     <row r="19" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
         <v>95</v>
-      </c>
-      <c r="B19" t="s">
-        <v>96</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" t="s">
@@ -29182,14 +29197,14 @@
         <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="s">
         <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -32145,7 +32160,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -32177,7 +32192,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -32201,7 +32216,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -32221,7 +32236,7 @@
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
@@ -32230,7 +32245,7 @@
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -32245,10 +32260,10 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
@@ -32260,7 +32275,7 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -35271,7 +35286,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -35303,7 +35318,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -35327,7 +35342,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -35347,7 +35362,7 @@
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
@@ -35356,7 +35371,7 @@
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
@@ -35371,7 +35386,7 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -35386,7 +35401,7 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -35399,24 +35414,23 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
         <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D8" s="3"/>
@@ -38413,10 +38427,10 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -38472,7 +38486,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -38484,12 +38498,12 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -38502,27 +38516,27 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
         <v>110</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -38540,7 +38554,7 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
@@ -38550,12 +38564,12 @@
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -38568,10 +38582,10 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" t="s">
         <v>117</v>
-      </c>
-      <c r="G7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -41569,7 +41583,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -41625,7 +41639,7 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -41637,12 +41651,12 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -41655,27 +41669,27 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
         <v>110</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
@@ -41693,7 +41707,7 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>45</v>
@@ -41703,12 +41717,12 @@
         <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -41721,10 +41735,10 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" t="s">
         <v>117</v>
-      </c>
-      <c r="G7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -44720,7 +44734,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.75" customWidth="1"/>
     <col min="2" max="2" width="17.25" customWidth="1"/>
@@ -44776,13 +44790,13 @@
     </row>
     <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>25</v>
@@ -44793,16 +44807,16 @@
     </row>
     <row r="3" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
         <v>110</v>
       </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -44810,7 +44824,7 @@
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -44819,7 +44833,7 @@
         <v>250</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -44827,13 +44841,13 @@
     </row>
     <row r="5" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
@@ -44841,7 +44855,7 @@
     </row>
     <row r="6" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -44850,7 +44864,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -44858,13 +44872,13 @@
     </row>
     <row r="7" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
         <v>26</v>

</xml_diff>